<commit_message>
add en edit scores leerkracht
</commit_message>
<xml_diff>
--- a/logboek.xlsx
+++ b/logboek.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aaron\Documents\git\school_platform\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED99F890-0881-4BC5-8A48-980EC3F6DADC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{883EA497-C19E-4232-862D-E50F2DD24D87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D5BD8C03-B50E-614E-91C7-1FD0568DB02A}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>Naam student 2:</t>
   </si>
@@ -67,6 +67,9 @@
   </si>
   <si>
     <t>Weergeven van score op toetsen pagina per student</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scores toevoegen en wijzigen door leerkracht(opeens error bij het inserten van scores) </t>
   </si>
 </sst>
 </file>
@@ -474,13 +477,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36EF922A-C188-1F43-B267-5D771EC01B6B}">
   <dimension ref="A1:D57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="61.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="73.25" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.875" customWidth="1"/>
     <col min="3" max="3" width="27.125" customWidth="1"/>
     <col min="4" max="4" width="27.5" customWidth="1"/>
@@ -567,9 +570,15 @@
       <c r="D7" s="7"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="8"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="7"/>
+      <c r="A8" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="6">
+        <v>45290</v>
+      </c>
+      <c r="C8" s="7">
+        <v>8</v>
+      </c>
       <c r="D8" s="7"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>